<commit_message>
Finalisation des mouvemnts de base du vaisseau et debut codage mouvement des astéroides
toutes les commandes de deplacement du vaisseau fonctionnent et se limitent bien aux bordures, les astéroides se dirigent bien en meme temps que les vaisseaux avec des threads QTimer et se réinitialise bien a la fin de leur course.
</commit_message>
<xml_diff>
--- a/Documentation/Fichiers personnels/CR_Matthew_Flenet.xlsx
+++ b/Documentation/Fichiers personnels/CR_Matthew_Flenet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA9FB85-54ED-4887-BBD4-4030150B32CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87A9A95-A481-4935-8688-8D94EBD61AAF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Compte Rendu - Matthew Flenet</t>
   </si>
@@ -67,9 +67,6 @@
     <t xml:space="preserve">confection de l'écran de jeu </t>
   </si>
   <si>
-    <t>codage desmouvemetns du vaisseau avec son importation</t>
-  </si>
-  <si>
     <t>début des bordures</t>
   </si>
   <si>
@@ -79,10 +76,28 @@
     <t>finition des bordures et test</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>1 heure 20 Minutes</t>
+  </si>
+  <si>
+    <t>codage des mouvements du vaisseau avec son importation</t>
+  </si>
+  <si>
+    <t>codage des mouvements du vaisseau</t>
+  </si>
+  <si>
+    <t>codage des parametres aléatoires ou non des astéroides</t>
+  </si>
+  <si>
+    <t>1 heure</t>
+  </si>
+  <si>
+    <t>2 heure</t>
+  </si>
+  <si>
+    <t>1 heure 30 minutes</t>
+  </si>
+  <si>
+    <t>codage des mouvements des astéroides, rectiligne,vertical</t>
   </si>
 </sst>
 </file>
@@ -284,6 +299,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -291,9 +309,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -589,7 +604,7 @@
   <dimension ref="B2:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,16 +613,17 @@
     <col min="3" max="3" width="80.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -662,7 +678,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="3"/>
       <c r="G6" s="3"/>
@@ -671,39 +687,39 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="20">
+      <c r="B7" s="17">
         <v>43777</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="20">
+      <c r="B8" s="17">
         <v>43777</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3"/>
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="20">
+      <c r="B9" s="17">
         <v>43777</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="E9" s="3"/>
     </row>
@@ -712,41 +728,67 @@
         <v>43784</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E10" s="16"/>
       <c r="I10" s="5"/>
       <c r="N10" s="5"/>
     </row>
     <row r="11" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="2"/>
+      <c r="B11" s="14">
+        <v>43784</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="16"/>
     </row>
     <row r="12" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="2"/>
+      <c r="B12" s="14">
+        <v>43784</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="16"/>
     </row>
     <row r="13" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="20"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="2"/>
+      <c r="B13" s="17">
+        <v>43798</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="2"/>
+      <c r="B14" s="17">
+        <v>43798</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
+      <c r="B15" s="17">
+        <v>43798</v>
+      </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="2"/>

</xml_diff>

<commit_message>
ajout d'un second astéroide et configuration de celui ci
</commit_message>
<xml_diff>
--- a/Documentation/Fichiers personnels/CR_Matthew_Flenet.xlsx
+++ b/Documentation/Fichiers personnels/CR_Matthew_Flenet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87A9A95-A481-4935-8688-8D94EBD61AAF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A218E8-67A3-4B1E-ABE8-640CD3A7C8F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Compte Rendu - Matthew Flenet</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>codage des mouvements des astéroides, rectiligne,vertical</t>
+  </si>
+  <si>
+    <t>Terminer les deplacements des 6 astéroides, 3 verticaux, 3 horizontaux</t>
+  </si>
+  <si>
+    <t>coder tout les parametres d'asteroide variable, position, taille …</t>
   </si>
 </sst>
 </file>
@@ -604,7 +610,7 @@
   <dimension ref="B2:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,6 +766,9 @@
         <v>20</v>
       </c>
       <c r="E12" s="16"/>
+      <c r="H12" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="17">
@@ -794,19 +803,27 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="14"/>
-      <c r="C16" s="10"/>
+      <c r="B16" s="14">
+        <v>43805</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="D16" s="10"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
+      <c r="B17" s="14">
+        <v>43805</v>
+      </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="14"/>
+      <c r="B18" s="14">
+        <v>43805</v>
+      </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="2"/>

</xml_diff>

<commit_message>
Finalisation du Projet, mise ajour detous les documents annexe et de quelques variables
</commit_message>
<xml_diff>
--- a/Documentation/Fichiers personnels/CR_Matthew_Flenet.xlsx
+++ b/Documentation/Fichiers personnels/CR_Matthew_Flenet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A218E8-67A3-4B1E-ABE8-640CD3A7C8F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72AFEF3-B3B3-462B-A01B-D27FFCEF71F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t>Compte Rendu - Matthew Flenet</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Création de ce document</t>
   </si>
   <si>
-    <t>10 minutes</t>
-  </si>
-  <si>
     <t>30 minutes</t>
   </si>
   <si>
@@ -73,18 +70,9 @@
     <t>20 minutes</t>
   </si>
   <si>
-    <t>finition des bordures et test</t>
-  </si>
-  <si>
-    <t>1 heure 20 Minutes</t>
-  </si>
-  <si>
     <t>codage des mouvements du vaisseau avec son importation</t>
   </si>
   <si>
-    <t>codage des mouvements du vaisseau</t>
-  </si>
-  <si>
     <t>codage des parametres aléatoires ou non des astéroides</t>
   </si>
   <si>
@@ -97,13 +85,79 @@
     <t>1 heure 30 minutes</t>
   </si>
   <si>
-    <t>codage des mouvements des astéroides, rectiligne,vertical</t>
-  </si>
-  <si>
-    <t>Terminer les deplacements des 6 astéroides, 3 verticaux, 3 horizontaux</t>
-  </si>
-  <si>
-    <t>coder tout les parametres d'asteroide variable, position, taille …</t>
+    <t>Ajout du dossier image du vaisseau pour l'interface graphique</t>
+  </si>
+  <si>
+    <t>5 minutes</t>
+  </si>
+  <si>
+    <t>Création de la page Game ou tout le jeu sera codé</t>
+  </si>
+  <si>
+    <t>Ajout des images (BackGround Hero, Asteroide…)</t>
+  </si>
+  <si>
+    <t>Mise en place déplacement du vaisseau a l'aide des commandes ui de l'interface grahique qt</t>
+  </si>
+  <si>
+    <t>Création Bordures et déplacements vaisseau</t>
+  </si>
+  <si>
+    <t>re-codage des mouvements du vaisseau</t>
+  </si>
+  <si>
+    <t>amélioration des mouvements du vaisseau</t>
+  </si>
+  <si>
+    <t>finition des bordures avec test</t>
+  </si>
+  <si>
+    <t>codage des mouvements d'un astéroides, rectiligne, vertical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coder un second astéroide avec les memes variables (sauf le départ pas au meme moment) </t>
+  </si>
+  <si>
+    <t>update du gitignore et rectification de nombreux problemes de merge</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>Grandes modifications générales (voir Github)</t>
+  </si>
+  <si>
+    <t>3H</t>
+  </si>
+  <si>
+    <t>Grandes modifications générales 2 (voir Github)</t>
+  </si>
+  <si>
+    <t>Grandes modifications générales 3 (voir Github)</t>
+  </si>
+  <si>
+    <t>Grandes modifications générales semi finale (voir Github)</t>
+  </si>
+  <si>
+    <t>1H</t>
+  </si>
+  <si>
+    <t>Finition du Programme avec recodage de l'envoi message serveur</t>
+  </si>
+  <si>
+    <t>Programme Fini, Test realisation du cahier de recette</t>
+  </si>
+  <si>
+    <t>20 Minutes</t>
+  </si>
+  <si>
+    <t>40 Minutes</t>
+  </si>
+  <si>
+    <t>15 minutes</t>
   </si>
 </sst>
 </file>
@@ -261,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -297,9 +351,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -609,27 +660,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="80.5703125" customWidth="1"/>
+    <col min="3" max="3" width="90" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="26.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -653,7 +705,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="E4" s="3"/>
       <c r="G4" s="7"/>
@@ -664,13 +716,13 @@
         <v>43756</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="G5" s="16"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="4" t="s">
         <v>5</v>
       </c>
@@ -681,10 +733,10 @@
         <v>43756</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="E6" s="3"/>
       <c r="G6" s="3"/>
@@ -693,249 +745,269 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="17">
+      <c r="B7" s="16">
         <v>43777</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="17">
+      <c r="B8" s="16">
         <v>43777</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="E8" s="3"/>
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17">
+      <c r="B9" s="16">
         <v>43777</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="15"/>
     </row>
     <row r="10" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="14">
-        <v>43784</v>
+      <c r="B10" s="16">
+        <v>43777</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="16"/>
+        <v>20</v>
+      </c>
+      <c r="E10" s="3"/>
       <c r="I10" s="5"/>
       <c r="N10" s="5"/>
     </row>
     <row r="11" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14">
+      <c r="B11" s="16">
+        <v>43777</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="16">
+        <v>43777</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="16">
+        <v>43777</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="16">
+        <v>43777</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="14">
         <v>43784</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="16"/>
-    </row>
-    <row r="12" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="14">
-        <v>43784</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="H12" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="17">
-        <v>43798</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="17">
-        <v>43798</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="17">
-        <v>43798</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="14">
-        <v>43805</v>
+        <v>43784</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="2"/>
+      <c r="D16" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
+        <v>43784</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="16">
+        <v>43798</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="16">
+        <v>43798</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="14">
         <v>43805</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="14">
+      <c r="C20" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="14">
         <v>43805</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="2"/>
+      <c r="C21" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="14"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="2"/>
+      <c r="B22" s="16">
+        <v>43811</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="14"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="2"/>
+      <c r="B23" s="16">
+        <v>43811</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="14"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="2"/>
+      <c r="B24" s="16">
+        <v>43811</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="15"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="2"/>
+      <c r="B25" s="14">
+        <v>43811</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="15"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="2"/>
+      <c r="B26" s="16">
+        <v>43812</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="3"/>
     </row>
     <row r="27" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="15"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="14"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="14"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="14"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="15"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="15"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="15"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="14"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="14"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="14"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="2"/>
-    </row>
+      <c r="B27" s="16">
+        <v>43812</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>

</xml_diff>

<commit_message>
Revert "Finalisation du Projet, mise ajour detous les documents annexe et de quelques variables"
This reverts commit ec642cfb7bbc92453b3d111cf29d02b61c588921.
</commit_message>
<xml_diff>
--- a/Documentation/Fichiers personnels/CR_Matthew_Flenet.xlsx
+++ b/Documentation/Fichiers personnels/CR_Matthew_Flenet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72AFEF3-B3B3-462B-A01B-D27FFCEF71F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A218E8-67A3-4B1E-ABE8-640CD3A7C8F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Compte Rendu - Matthew Flenet</t>
   </si>
@@ -52,6 +52,9 @@
     <t>Création de ce document</t>
   </si>
   <si>
+    <t>10 minutes</t>
+  </si>
+  <si>
     <t>30 minutes</t>
   </si>
   <si>
@@ -70,9 +73,18 @@
     <t>20 minutes</t>
   </si>
   <si>
+    <t>finition des bordures et test</t>
+  </si>
+  <si>
+    <t>1 heure 20 Minutes</t>
+  </si>
+  <si>
     <t>codage des mouvements du vaisseau avec son importation</t>
   </si>
   <si>
+    <t>codage des mouvements du vaisseau</t>
+  </si>
+  <si>
     <t>codage des parametres aléatoires ou non des astéroides</t>
   </si>
   <si>
@@ -85,79 +97,13 @@
     <t>1 heure 30 minutes</t>
   </si>
   <si>
-    <t>Ajout du dossier image du vaisseau pour l'interface graphique</t>
-  </si>
-  <si>
-    <t>5 minutes</t>
-  </si>
-  <si>
-    <t>Création de la page Game ou tout le jeu sera codé</t>
-  </si>
-  <si>
-    <t>Ajout des images (BackGround Hero, Asteroide…)</t>
-  </si>
-  <si>
-    <t>Mise en place déplacement du vaisseau a l'aide des commandes ui de l'interface grahique qt</t>
-  </si>
-  <si>
-    <t>Création Bordures et déplacements vaisseau</t>
-  </si>
-  <si>
-    <t>re-codage des mouvements du vaisseau</t>
-  </si>
-  <si>
-    <t>amélioration des mouvements du vaisseau</t>
-  </si>
-  <si>
-    <t>finition des bordures avec test</t>
-  </si>
-  <si>
-    <t>codage des mouvements d'un astéroides, rectiligne, vertical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coder un second astéroide avec les memes variables (sauf le départ pas au meme moment) </t>
-  </si>
-  <si>
-    <t>update du gitignore et rectification de nombreux problemes de merge</t>
-  </si>
-  <si>
-    <t>1h</t>
-  </si>
-  <si>
-    <t>2h</t>
-  </si>
-  <si>
-    <t>Grandes modifications générales (voir Github)</t>
-  </si>
-  <si>
-    <t>3H</t>
-  </si>
-  <si>
-    <t>Grandes modifications générales 2 (voir Github)</t>
-  </si>
-  <si>
-    <t>Grandes modifications générales 3 (voir Github)</t>
-  </si>
-  <si>
-    <t>Grandes modifications générales semi finale (voir Github)</t>
-  </si>
-  <si>
-    <t>1H</t>
-  </si>
-  <si>
-    <t>Finition du Programme avec recodage de l'envoi message serveur</t>
-  </si>
-  <si>
-    <t>Programme Fini, Test realisation du cahier de recette</t>
-  </si>
-  <si>
-    <t>20 Minutes</t>
-  </si>
-  <si>
-    <t>40 Minutes</t>
-  </si>
-  <si>
-    <t>15 minutes</t>
+    <t>codage des mouvements des astéroides, rectiligne,vertical</t>
+  </si>
+  <si>
+    <t>Terminer les deplacements des 6 astéroides, 3 verticaux, 3 horizontaux</t>
+  </si>
+  <si>
+    <t>coder tout les parametres d'asteroide variable, position, taille …</t>
   </si>
 </sst>
 </file>
@@ -315,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -351,6 +297,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -660,28 +609,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="90" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="26.28515625" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -705,7 +653,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3"/>
       <c r="G4" s="7"/>
@@ -716,13 +664,13 @@
         <v>43756</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="G5" s="15"/>
+      <c r="G5" s="16"/>
       <c r="H5" s="4" t="s">
         <v>5</v>
       </c>
@@ -733,10 +681,10 @@
         <v>43756</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="E6" s="3"/>
       <c r="G6" s="3"/>
@@ -745,269 +693,249 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
+      <c r="B7" s="17">
         <v>43777</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
+      <c r="B8" s="17">
         <v>43777</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3"/>
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16">
+      <c r="B9" s="17">
         <v>43777</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="15"/>
+        <v>14</v>
+      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16">
-        <v>43777</v>
+      <c r="B10" s="14">
+        <v>43784</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="E10" s="16"/>
       <c r="I10" s="5"/>
       <c r="N10" s="5"/>
     </row>
     <row r="11" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16">
-        <v>43777</v>
+      <c r="B11" s="14">
+        <v>43784</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="14">
+        <v>43784</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16">
-        <v>43777</v>
-      </c>
-      <c r="C12" s="10" t="s">
+      <c r="E12" s="16"/>
+      <c r="H12" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="17">
+        <v>43798</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="17">
+        <v>43798</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16">
-        <v>43777</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="15"/>
-    </row>
-    <row r="14" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="16">
-        <v>43777</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="14">
-        <v>43784</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="3"/>
+      <c r="B15" s="17">
+        <v>43798</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="14">
-        <v>43784</v>
+        <v>43805</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="3"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
-        <v>43784</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="15"/>
+        <v>43805</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="16">
-        <v>43798</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="3"/>
+      <c r="B18" s="14">
+        <v>43805</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="16">
-        <v>43798</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="3"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="14">
-        <v>43805</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="3"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="14">
-        <v>43805</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="3"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="16">
-        <v>43811</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="3"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="16">
-        <v>43811</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="3"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="16">
-        <v>43811</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="3"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="14">
-        <v>43811</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" s="3"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="16">
-        <v>43812</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E26" s="3"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="16">
-        <v>43812</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="14"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="14"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="14"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="15"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="15"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="15"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="14"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="14"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="14"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="2"/>
+    </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>

</xml_diff>